<commit_message>
Downgrading to xlsx version 0.7.12
</commit_message>
<xml_diff>
--- a/test/examples/sheet.xlsx
+++ b/test/examples/sheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr date1904="false"/>
   <sheets>
     <sheet name="SheetJS" sheetId="1" r:id="rId1"/>
   </sheets>
@@ -10,9 +10,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -376,9 +373,6 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -404,54 +398,51 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="str">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="str">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="str">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="str">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="str">
         <v>6</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="str">
         <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" t="str">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="str">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="str">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="str">
         <v>6</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="str">
         <v>7</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="str">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>